<commit_message>
impact of earnings vol quartile model
</commit_message>
<xml_diff>
--- a/content/post/data/ABS_Weekly_data.xlsx
+++ b/content/post/data/ABS_Weekly_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atroyer\Documents\Projects\insurer-valuation-study\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atroyer\Documents\Projects\problemofpoints\content\post\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -8297,7 +8297,7 @@
         <v>30.2</v>
       </c>
       <c r="AG60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:33" x14ac:dyDescent="0.25">
@@ -14140,7 +14140,7 @@
         <v>11.3</v>
       </c>
       <c r="AG122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="2:33" x14ac:dyDescent="0.25">

</xml_diff>